<commit_message>
chore: add staffing_real and sale_plan new data
</commit_message>
<xml_diff>
--- a/lib/tasks/data/staffing_real.xlsx
+++ b/lib/tasks/data/staffing_real.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="StaffingReal" sheetId="1" state="visible" r:id="rId2"/>
@@ -170,8 +170,8 @@
   </sheetPr>
   <dimension ref="A1:G303"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A273" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H273" activeCellId="0" sqref="H273"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2297,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G92" s="0" t="n">
         <v>1</v>
@@ -2320,7 +2320,7 @@
         <v>2</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="G93" s="0" t="n">
         <v>1</v>
@@ -2343,7 +2343,7 @@
         <v>3</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="G94" s="0" t="n">
         <v>1</v>
@@ -2366,7 +2366,7 @@
         <v>4</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="G95" s="0" t="n">
         <v>1</v>
@@ -2389,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G96" s="0" t="n">
         <v>1</v>
@@ -2412,7 +2412,7 @@
         <v>6</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G97" s="0" t="n">
         <v>1</v>
@@ -2435,7 +2435,7 @@
         <v>7</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G98" s="0" t="n">
         <v>1</v>
@@ -2458,7 +2458,7 @@
         <v>8</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="G99" s="0" t="n">
         <v>1</v>
@@ -2481,7 +2481,7 @@
         <v>9</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="G100" s="0" t="n">
         <v>1</v>
@@ -2504,7 +2504,7 @@
         <v>10</v>
       </c>
       <c r="F101" s="0" t="n">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="G101" s="0" t="n">
         <v>1</v>
@@ -2527,7 +2527,7 @@
         <v>11</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G102" s="0" t="n">
         <v>1</v>
@@ -2550,7 +2550,7 @@
         <v>12</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="G103" s="0" t="n">
         <v>1</v>
@@ -2573,7 +2573,7 @@
         <v>13</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G104" s="0" t="n">
         <v>1</v>
@@ -2596,7 +2596,7 @@
         <v>14</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>1</v>
@@ -2619,7 +2619,7 @@
         <v>15</v>
       </c>
       <c r="F106" s="0" t="n">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>1</v>
@@ -2642,7 +2642,7 @@
         <v>16</v>
       </c>
       <c r="F107" s="0" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>1</v>
@@ -2665,7 +2665,7 @@
         <v>17</v>
       </c>
       <c r="F108" s="0" t="n">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="G108" s="0" t="n">
         <v>1</v>
@@ -2688,7 +2688,7 @@
         <v>18</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G109" s="0" t="n">
         <v>1</v>
@@ -2711,7 +2711,7 @@
         <v>19</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="G110" s="0" t="n">
         <v>1</v>
@@ -2734,7 +2734,7 @@
         <v>20</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="G111" s="0" t="n">
         <v>1</v>
@@ -2757,7 +2757,7 @@
         <v>21</v>
       </c>
       <c r="F112" s="0" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G112" s="0" t="n">
         <v>1</v>
@@ -2780,7 +2780,7 @@
         <v>22</v>
       </c>
       <c r="F113" s="0" t="n">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="G113" s="0" t="n">
         <v>1</v>
@@ -2826,7 +2826,7 @@
         <v>24</v>
       </c>
       <c r="F115" s="0" t="n">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="G115" s="0" t="n">
         <v>1</v>
@@ -2849,7 +2849,7 @@
         <v>25</v>
       </c>
       <c r="F116" s="0" t="n">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="G116" s="0" t="n">
         <v>1</v>
@@ -2872,7 +2872,7 @@
         <v>26</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="G117" s="0" t="n">
         <v>1</v>
@@ -2895,7 +2895,7 @@
         <v>27</v>
       </c>
       <c r="F118" s="0" t="n">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="G118" s="0" t="n">
         <v>1</v>
@@ -2918,7 +2918,7 @@
         <v>28</v>
       </c>
       <c r="F119" s="0" t="n">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="G119" s="0" t="n">
         <v>1</v>
@@ -2941,7 +2941,7 @@
         <v>29</v>
       </c>
       <c r="F120" s="0" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G120" s="0" t="n">
         <v>1</v>
@@ -2964,7 +2964,7 @@
         <v>30</v>
       </c>
       <c r="F121" s="0" t="n">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="G121" s="0" t="n">
         <v>1</v>
@@ -2987,7 +2987,7 @@
         <v>1</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="G122" s="0" t="n">
         <v>1</v>
@@ -3010,7 +3010,7 @@
         <v>2</v>
       </c>
       <c r="F123" s="0" t="n">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="G123" s="0" t="n">
         <v>1</v>
@@ -3033,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="F124" s="0" t="n">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="G124" s="0" t="n">
         <v>1</v>
@@ -3056,7 +3056,7 @@
         <v>4</v>
       </c>
       <c r="F125" s="0" t="n">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="G125" s="0" t="n">
         <v>1</v>
@@ -3079,7 +3079,7 @@
         <v>5</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="G126" s="0" t="n">
         <v>1</v>
@@ -3102,7 +3102,7 @@
         <v>6</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="G127" s="0" t="n">
         <v>1</v>
@@ -3125,7 +3125,7 @@
         <v>7</v>
       </c>
       <c r="F128" s="0" t="n">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G128" s="0" t="n">
         <v>1</v>
@@ -3148,7 +3148,7 @@
         <v>8</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="G129" s="0" t="n">
         <v>1</v>
@@ -3171,7 +3171,7 @@
         <v>9</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="G130" s="0" t="n">
         <v>1</v>
@@ -3194,7 +3194,7 @@
         <v>10</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="G131" s="0" t="n">
         <v>1</v>
@@ -3217,7 +3217,7 @@
         <v>11</v>
       </c>
       <c r="F132" s="0" t="n">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="G132" s="0" t="n">
         <v>1</v>
@@ -3240,7 +3240,7 @@
         <v>12</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="G133" s="0" t="n">
         <v>1</v>
@@ -3263,7 +3263,7 @@
         <v>13</v>
       </c>
       <c r="F134" s="0" t="n">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G134" s="0" t="n">
         <v>1</v>
@@ -3286,7 +3286,7 @@
         <v>14</v>
       </c>
       <c r="F135" s="0" t="n">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="G135" s="0" t="n">
         <v>1</v>
@@ -3309,7 +3309,7 @@
         <v>15</v>
       </c>
       <c r="F136" s="0" t="n">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="G136" s="0" t="n">
         <v>1</v>
@@ -3332,7 +3332,7 @@
         <v>16</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G137" s="0" t="n">
         <v>1</v>
@@ -3355,7 +3355,7 @@
         <v>17</v>
       </c>
       <c r="F138" s="0" t="n">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="G138" s="0" t="n">
         <v>1</v>
@@ -3378,7 +3378,7 @@
         <v>18</v>
       </c>
       <c r="F139" s="0" t="n">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="G139" s="0" t="n">
         <v>1</v>
@@ -3401,7 +3401,7 @@
         <v>19</v>
       </c>
       <c r="F140" s="0" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="G140" s="0" t="n">
         <v>1</v>
@@ -3424,7 +3424,7 @@
         <v>20</v>
       </c>
       <c r="F141" s="0" t="n">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="G141" s="0" t="n">
         <v>1</v>
@@ -3447,7 +3447,7 @@
         <v>21</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="G142" s="0" t="n">
         <v>1</v>
@@ -3470,7 +3470,7 @@
         <v>22</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="G143" s="0" t="n">
         <v>1</v>
@@ -3493,7 +3493,7 @@
         <v>23</v>
       </c>
       <c r="F144" s="0" t="n">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="G144" s="0" t="n">
         <v>1</v>
@@ -3516,7 +3516,7 @@
         <v>24</v>
       </c>
       <c r="F145" s="0" t="n">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="G145" s="0" t="n">
         <v>1</v>
@@ -3539,7 +3539,7 @@
         <v>25</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="G146" s="0" t="n">
         <v>1</v>
@@ -3562,7 +3562,7 @@
         <v>26</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="G147" s="0" t="n">
         <v>1</v>
@@ -3585,7 +3585,7 @@
         <v>27</v>
       </c>
       <c r="F148" s="0" t="n">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="G148" s="0" t="n">
         <v>1</v>
@@ -3608,7 +3608,7 @@
         <v>28</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="G149" s="0" t="n">
         <v>1</v>
@@ -3631,7 +3631,7 @@
         <v>29</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>83</v>
+        <v>138</v>
       </c>
       <c r="G150" s="0" t="n">
         <v>1</v>
@@ -3654,7 +3654,7 @@
         <v>30</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="G151" s="0" t="n">
         <v>1</v>
@@ -3677,7 +3677,7 @@
         <v>31</v>
       </c>
       <c r="F152" s="0" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G152" s="0" t="n">
         <v>1</v>
@@ -6460,7 +6460,7 @@
         <v>1</v>
       </c>
       <c r="F273" s="0" t="n">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G273" s="0" t="n">
         <v>1</v>
@@ -6483,7 +6483,7 @@
         <v>2</v>
       </c>
       <c r="F274" s="0" t="n">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="G274" s="0" t="n">
         <v>1</v>
@@ -6506,7 +6506,7 @@
         <v>3</v>
       </c>
       <c r="F275" s="0" t="n">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="G275" s="0" t="n">
         <v>1</v>
@@ -6529,7 +6529,7 @@
         <v>4</v>
       </c>
       <c r="F276" s="0" t="n">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="G276" s="0" t="n">
         <v>1</v>
@@ -6552,7 +6552,7 @@
         <v>5</v>
       </c>
       <c r="F277" s="0" t="n">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="G277" s="0" t="n">
         <v>1</v>
@@ -6575,7 +6575,7 @@
         <v>6</v>
       </c>
       <c r="F278" s="0" t="n">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="G278" s="0" t="n">
         <v>1</v>
@@ -6598,7 +6598,7 @@
         <v>7</v>
       </c>
       <c r="F279" s="0" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G279" s="0" t="n">
         <v>1</v>
@@ -6621,7 +6621,7 @@
         <v>8</v>
       </c>
       <c r="F280" s="0" t="n">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="G280" s="0" t="n">
         <v>1</v>
@@ -6644,7 +6644,7 @@
         <v>9</v>
       </c>
       <c r="F281" s="0" t="n">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="G281" s="0" t="n">
         <v>1</v>
@@ -6667,7 +6667,7 @@
         <v>10</v>
       </c>
       <c r="F282" s="0" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G282" s="0" t="n">
         <v>1</v>
@@ -6690,7 +6690,7 @@
         <v>11</v>
       </c>
       <c r="F283" s="0" t="n">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="G283" s="0" t="n">
         <v>1</v>
@@ -6713,7 +6713,7 @@
         <v>12</v>
       </c>
       <c r="F284" s="0" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G284" s="0" t="n">
         <v>1</v>
@@ -6736,7 +6736,7 @@
         <v>13</v>
       </c>
       <c r="F285" s="0" t="n">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G285" s="0" t="n">
         <v>1</v>
@@ -6759,7 +6759,7 @@
         <v>14</v>
       </c>
       <c r="F286" s="0" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="G286" s="0" t="n">
         <v>1</v>
@@ -6782,7 +6782,7 @@
         <v>15</v>
       </c>
       <c r="F287" s="0" t="n">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="G287" s="0" t="n">
         <v>1</v>
@@ -6805,7 +6805,7 @@
         <v>16</v>
       </c>
       <c r="F288" s="0" t="n">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G288" s="0" t="n">
         <v>1</v>
@@ -6828,7 +6828,7 @@
         <v>17</v>
       </c>
       <c r="F289" s="0" t="n">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="G289" s="0" t="n">
         <v>1</v>
@@ -6851,7 +6851,7 @@
         <v>18</v>
       </c>
       <c r="F290" s="0" t="n">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="G290" s="0" t="n">
         <v>1</v>
@@ -6874,7 +6874,7 @@
         <v>19</v>
       </c>
       <c r="F291" s="0" t="n">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="G291" s="0" t="n">
         <v>1</v>
@@ -6897,7 +6897,7 @@
         <v>20</v>
       </c>
       <c r="F292" s="0" t="n">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="G292" s="0" t="n">
         <v>1</v>
@@ -6920,7 +6920,7 @@
         <v>21</v>
       </c>
       <c r="F293" s="0" t="n">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="G293" s="0" t="n">
         <v>1</v>
@@ -6943,7 +6943,7 @@
         <v>22</v>
       </c>
       <c r="F294" s="0" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G294" s="0" t="n">
         <v>1</v>
@@ -6966,7 +6966,7 @@
         <v>23</v>
       </c>
       <c r="F295" s="0" t="n">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="G295" s="0" t="n">
         <v>1</v>
@@ -6989,7 +6989,7 @@
         <v>24</v>
       </c>
       <c r="F296" s="0" t="n">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="G296" s="0" t="n">
         <v>1</v>
@@ -7012,7 +7012,7 @@
         <v>25</v>
       </c>
       <c r="F297" s="0" t="n">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G297" s="0" t="n">
         <v>1</v>
@@ -7035,7 +7035,7 @@
         <v>26</v>
       </c>
       <c r="F298" s="0" t="n">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="G298" s="0" t="n">
         <v>1</v>
@@ -7058,7 +7058,7 @@
         <v>27</v>
       </c>
       <c r="F299" s="0" t="n">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="G299" s="0" t="n">
         <v>1</v>
@@ -7081,7 +7081,7 @@
         <v>28</v>
       </c>
       <c r="F300" s="0" t="n">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="G300" s="0" t="n">
         <v>1</v>
@@ -7104,7 +7104,7 @@
         <v>29</v>
       </c>
       <c r="F301" s="0" t="n">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="G301" s="0" t="n">
         <v>1</v>
@@ -7127,7 +7127,7 @@
         <v>30</v>
       </c>
       <c r="F302" s="0" t="n">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="G302" s="0" t="n">
         <v>1</v>
@@ -7150,7 +7150,7 @@
         <v>31</v>
       </c>
       <c r="F303" s="0" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G303" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
improve érformace of query to available_shit
</commit_message>
<xml_diff>
--- a/lib/tasks/data/staffing_real.xlsx
+++ b/lib/tasks/data/staffing_real.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="StaffingReal" sheetId="1" state="visible" r:id="rId2"/>
@@ -2297,7 +2297,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G92" s="0" t="n">
         <v>1</v>
@@ -2320,7 +2320,7 @@
         <v>2</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G93" s="0" t="n">
         <v>1</v>
@@ -2343,7 +2343,7 @@
         <v>3</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="G94" s="0" t="n">
         <v>1</v>
@@ -2366,7 +2366,7 @@
         <v>4</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G95" s="0" t="n">
         <v>1</v>
@@ -2389,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G96" s="0" t="n">
         <v>1</v>
@@ -2412,7 +2412,7 @@
         <v>6</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G97" s="0" t="n">
         <v>1</v>
@@ -2435,7 +2435,7 @@
         <v>7</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G98" s="0" t="n">
         <v>1</v>
@@ -2458,7 +2458,7 @@
         <v>8</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G99" s="0" t="n">
         <v>1</v>
@@ -2481,7 +2481,7 @@
         <v>9</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="G100" s="0" t="n">
         <v>1</v>
@@ -2504,7 +2504,7 @@
         <v>10</v>
       </c>
       <c r="F101" s="0" t="n">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="G101" s="0" t="n">
         <v>1</v>
@@ -2527,7 +2527,7 @@
         <v>11</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G102" s="0" t="n">
         <v>1</v>
@@ -2550,7 +2550,7 @@
         <v>12</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G103" s="0" t="n">
         <v>1</v>
@@ -2573,7 +2573,7 @@
         <v>13</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G104" s="0" t="n">
         <v>1</v>
@@ -2596,7 +2596,7 @@
         <v>14</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>1</v>
@@ -2619,7 +2619,7 @@
         <v>15</v>
       </c>
       <c r="F106" s="0" t="n">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>1</v>
@@ -2642,7 +2642,7 @@
         <v>16</v>
       </c>
       <c r="F107" s="0" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>1</v>
@@ -2665,7 +2665,7 @@
         <v>17</v>
       </c>
       <c r="F108" s="0" t="n">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G108" s="0" t="n">
         <v>1</v>
@@ -2688,7 +2688,7 @@
         <v>18</v>
       </c>
       <c r="F109" s="0" t="n">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G109" s="0" t="n">
         <v>1</v>
@@ -2711,7 +2711,7 @@
         <v>19</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G110" s="0" t="n">
         <v>1</v>
@@ -2734,7 +2734,7 @@
         <v>20</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G111" s="0" t="n">
         <v>1</v>
@@ -2757,7 +2757,7 @@
         <v>21</v>
       </c>
       <c r="F112" s="0" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G112" s="0" t="n">
         <v>1</v>
@@ -2780,7 +2780,7 @@
         <v>22</v>
       </c>
       <c r="F113" s="0" t="n">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="G113" s="0" t="n">
         <v>1</v>
@@ -2826,7 +2826,7 @@
         <v>24</v>
       </c>
       <c r="F115" s="0" t="n">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="G115" s="0" t="n">
         <v>1</v>
@@ -2849,7 +2849,7 @@
         <v>25</v>
       </c>
       <c r="F116" s="0" t="n">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="G116" s="0" t="n">
         <v>1</v>
@@ -2872,7 +2872,7 @@
         <v>26</v>
       </c>
       <c r="F117" s="0" t="n">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G117" s="0" t="n">
         <v>1</v>
@@ -2895,7 +2895,7 @@
         <v>27</v>
       </c>
       <c r="F118" s="0" t="n">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G118" s="0" t="n">
         <v>1</v>
@@ -2918,7 +2918,7 @@
         <v>28</v>
       </c>
       <c r="F119" s="0" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="G119" s="0" t="n">
         <v>1</v>
@@ -2941,7 +2941,7 @@
         <v>29</v>
       </c>
       <c r="F120" s="0" t="n">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G120" s="0" t="n">
         <v>1</v>
@@ -2964,7 +2964,7 @@
         <v>30</v>
       </c>
       <c r="F121" s="0" t="n">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G121" s="0" t="n">
         <v>1</v>
@@ -2987,7 +2987,7 @@
         <v>1</v>
       </c>
       <c r="F122" s="0" t="n">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="G122" s="0" t="n">
         <v>1</v>
@@ -3010,7 +3010,7 @@
         <v>2</v>
       </c>
       <c r="F123" s="0" t="n">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="G123" s="0" t="n">
         <v>1</v>
@@ -3033,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="F124" s="0" t="n">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="G124" s="0" t="n">
         <v>1</v>
@@ -3056,7 +3056,7 @@
         <v>4</v>
       </c>
       <c r="F125" s="0" t="n">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="G125" s="0" t="n">
         <v>1</v>
@@ -3079,7 +3079,7 @@
         <v>5</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="G126" s="0" t="n">
         <v>1</v>
@@ -3102,7 +3102,7 @@
         <v>6</v>
       </c>
       <c r="F127" s="0" t="n">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G127" s="0" t="n">
         <v>1</v>
@@ -3125,7 +3125,7 @@
         <v>7</v>
       </c>
       <c r="F128" s="0" t="n">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="G128" s="0" t="n">
         <v>1</v>
@@ -3148,7 +3148,7 @@
         <v>8</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="G129" s="0" t="n">
         <v>1</v>
@@ -3171,7 +3171,7 @@
         <v>9</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="G130" s="0" t="n">
         <v>1</v>
@@ -3194,7 +3194,7 @@
         <v>10</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G131" s="0" t="n">
         <v>1</v>
@@ -3217,7 +3217,7 @@
         <v>11</v>
       </c>
       <c r="F132" s="0" t="n">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="G132" s="0" t="n">
         <v>1</v>
@@ -3240,7 +3240,7 @@
         <v>12</v>
       </c>
       <c r="F133" s="0" t="n">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="G133" s="0" t="n">
         <v>1</v>
@@ -3263,7 +3263,7 @@
         <v>13</v>
       </c>
       <c r="F134" s="0" t="n">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G134" s="0" t="n">
         <v>1</v>
@@ -3286,7 +3286,7 @@
         <v>14</v>
       </c>
       <c r="F135" s="0" t="n">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="G135" s="0" t="n">
         <v>1</v>
@@ -3309,7 +3309,7 @@
         <v>15</v>
       </c>
       <c r="F136" s="0" t="n">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="G136" s="0" t="n">
         <v>1</v>
@@ -3332,7 +3332,7 @@
         <v>16</v>
       </c>
       <c r="F137" s="0" t="n">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G137" s="0" t="n">
         <v>1</v>
@@ -3355,7 +3355,7 @@
         <v>17</v>
       </c>
       <c r="F138" s="0" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="G138" s="0" t="n">
         <v>1</v>
@@ -3378,7 +3378,7 @@
         <v>18</v>
       </c>
       <c r="F139" s="0" t="n">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="G139" s="0" t="n">
         <v>1</v>
@@ -3401,7 +3401,7 @@
         <v>19</v>
       </c>
       <c r="F140" s="0" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G140" s="0" t="n">
         <v>1</v>
@@ -3424,7 +3424,7 @@
         <v>20</v>
       </c>
       <c r="F141" s="0" t="n">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="G141" s="0" t="n">
         <v>1</v>
@@ -3447,7 +3447,7 @@
         <v>21</v>
       </c>
       <c r="F142" s="0" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="G142" s="0" t="n">
         <v>1</v>
@@ -3470,7 +3470,7 @@
         <v>22</v>
       </c>
       <c r="F143" s="0" t="n">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="G143" s="0" t="n">
         <v>1</v>
@@ -3493,7 +3493,7 @@
         <v>23</v>
       </c>
       <c r="F144" s="0" t="n">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="G144" s="0" t="n">
         <v>1</v>
@@ -3516,7 +3516,7 @@
         <v>24</v>
       </c>
       <c r="F145" s="0" t="n">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="G145" s="0" t="n">
         <v>1</v>
@@ -3539,7 +3539,7 @@
         <v>25</v>
       </c>
       <c r="F146" s="0" t="n">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="G146" s="0" t="n">
         <v>1</v>
@@ -3562,7 +3562,7 @@
         <v>26</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="G147" s="0" t="n">
         <v>1</v>
@@ -3585,7 +3585,7 @@
         <v>27</v>
       </c>
       <c r="F148" s="0" t="n">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="G148" s="0" t="n">
         <v>1</v>
@@ -3608,7 +3608,7 @@
         <v>28</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="G149" s="0" t="n">
         <v>1</v>
@@ -3631,7 +3631,7 @@
         <v>29</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>138</v>
+        <v>83</v>
       </c>
       <c r="G150" s="0" t="n">
         <v>1</v>
@@ -3654,7 +3654,7 @@
         <v>30</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G151" s="0" t="n">
         <v>1</v>
@@ -3677,7 +3677,7 @@
         <v>31</v>
       </c>
       <c r="F152" s="0" t="n">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="G152" s="0" t="n">
         <v>1</v>
@@ -3907,7 +3907,7 @@
         <v>10</v>
       </c>
       <c r="F162" s="0" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G162" s="0" t="n">
         <v>1</v>
@@ -4919,7 +4919,7 @@
         <v>23</v>
       </c>
       <c r="F206" s="0" t="n">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="G206" s="0" t="n">
         <v>1</v>
@@ -6460,7 +6460,7 @@
         <v>1</v>
       </c>
       <c r="F273" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G273" s="0" t="n">
         <v>1</v>
@@ -6483,7 +6483,7 @@
         <v>2</v>
       </c>
       <c r="F274" s="0" t="n">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G274" s="0" t="n">
         <v>1</v>
@@ -6506,7 +6506,7 @@
         <v>3</v>
       </c>
       <c r="F275" s="0" t="n">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="G275" s="0" t="n">
         <v>1</v>
@@ -6529,7 +6529,7 @@
         <v>4</v>
       </c>
       <c r="F276" s="0" t="n">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="G276" s="0" t="n">
         <v>1</v>
@@ -6552,7 +6552,7 @@
         <v>5</v>
       </c>
       <c r="F277" s="0" t="n">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="G277" s="0" t="n">
         <v>1</v>
@@ -6575,7 +6575,7 @@
         <v>6</v>
       </c>
       <c r="F278" s="0" t="n">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G278" s="0" t="n">
         <v>1</v>
@@ -6598,7 +6598,7 @@
         <v>7</v>
       </c>
       <c r="F279" s="0" t="n">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G279" s="0" t="n">
         <v>1</v>
@@ -6621,7 +6621,7 @@
         <v>8</v>
       </c>
       <c r="F280" s="0" t="n">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G280" s="0" t="n">
         <v>1</v>
@@ -6644,7 +6644,7 @@
         <v>9</v>
       </c>
       <c r="F281" s="0" t="n">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="G281" s="0" t="n">
         <v>1</v>
@@ -6667,7 +6667,7 @@
         <v>10</v>
       </c>
       <c r="F282" s="0" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G282" s="0" t="n">
         <v>1</v>
@@ -6690,7 +6690,7 @@
         <v>11</v>
       </c>
       <c r="F283" s="0" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G283" s="0" t="n">
         <v>1</v>
@@ -6713,7 +6713,7 @@
         <v>12</v>
       </c>
       <c r="F284" s="0" t="n">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="G284" s="0" t="n">
         <v>1</v>
@@ -6736,7 +6736,7 @@
         <v>13</v>
       </c>
       <c r="F285" s="0" t="n">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G285" s="0" t="n">
         <v>1</v>
@@ -6759,7 +6759,7 @@
         <v>14</v>
       </c>
       <c r="F286" s="0" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="G286" s="0" t="n">
         <v>1</v>
@@ -6782,7 +6782,7 @@
         <v>15</v>
       </c>
       <c r="F287" s="0" t="n">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="G287" s="0" t="n">
         <v>1</v>
@@ -6805,7 +6805,7 @@
         <v>16</v>
       </c>
       <c r="F288" s="0" t="n">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G288" s="0" t="n">
         <v>1</v>
@@ -6828,7 +6828,7 @@
         <v>17</v>
       </c>
       <c r="F289" s="0" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="G289" s="0" t="n">
         <v>1</v>
@@ -6851,7 +6851,7 @@
         <v>18</v>
       </c>
       <c r="F290" s="0" t="n">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G290" s="0" t="n">
         <v>1</v>
@@ -6874,7 +6874,7 @@
         <v>19</v>
       </c>
       <c r="F291" s="0" t="n">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G291" s="0" t="n">
         <v>1</v>
@@ -6897,7 +6897,7 @@
         <v>20</v>
       </c>
       <c r="F292" s="0" t="n">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="G292" s="0" t="n">
         <v>1</v>
@@ -6920,7 +6920,7 @@
         <v>21</v>
       </c>
       <c r="F293" s="0" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="G293" s="0" t="n">
         <v>1</v>
@@ -6943,7 +6943,7 @@
         <v>22</v>
       </c>
       <c r="F294" s="0" t="n">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G294" s="0" t="n">
         <v>1</v>
@@ -6966,7 +6966,7 @@
         <v>23</v>
       </c>
       <c r="F295" s="0" t="n">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G295" s="0" t="n">
         <v>1</v>
@@ -6989,7 +6989,7 @@
         <v>24</v>
       </c>
       <c r="F296" s="0" t="n">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="G296" s="0" t="n">
         <v>1</v>
@@ -7012,7 +7012,7 @@
         <v>25</v>
       </c>
       <c r="F297" s="0" t="n">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G297" s="0" t="n">
         <v>1</v>
@@ -7035,7 +7035,7 @@
         <v>26</v>
       </c>
       <c r="F298" s="0" t="n">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="G298" s="0" t="n">
         <v>1</v>
@@ -7058,7 +7058,7 @@
         <v>27</v>
       </c>
       <c r="F299" s="0" t="n">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="G299" s="0" t="n">
         <v>1</v>
@@ -7081,7 +7081,7 @@
         <v>28</v>
       </c>
       <c r="F300" s="0" t="n">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="G300" s="0" t="n">
         <v>1</v>
@@ -7104,7 +7104,7 @@
         <v>29</v>
       </c>
       <c r="F301" s="0" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="G301" s="0" t="n">
         <v>1</v>
@@ -7127,7 +7127,7 @@
         <v>30</v>
       </c>
       <c r="F302" s="0" t="n">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="G302" s="0" t="n">
         <v>1</v>
@@ -7150,7 +7150,7 @@
         <v>31</v>
       </c>
       <c r="F303" s="0" t="n">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="G303" s="0" t="n">
         <v>1</v>

</xml_diff>